<commit_message>
Code update july 8th
</commit_message>
<xml_diff>
--- a/ponderacion_modelos.xlsx
+++ b/ponderacion_modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malfaro\Desktop\mae_code\House_price_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966A45E0-AE38-4DED-95C2-013EC70C0F30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE3EF52-FF53-4AE1-8EE3-D1E0DB7543EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14785086-4257-45D9-9F19-8FF5E0E725A2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
   <si>
     <t>lightgbm</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>data_0</t>
+  </si>
+  <si>
+    <t>all_2</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F149A9AD-B57D-46C1-8C8B-66C5A0940566}">
-  <dimension ref="B3:O53"/>
+  <dimension ref="B3:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="P62" sqref="P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +817,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="33" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K33" t="s">
         <v>8</v>
       </c>
@@ -822,7 +825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="M34" s="1" t="s">
         <v>2</v>
       </c>
@@ -833,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="M35" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +847,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="M36" s="1" t="s">
         <v>1</v>
       </c>
@@ -855,7 +858,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
       <c r="M37" s="1" t="s">
         <v>3</v>
       </c>
@@ -866,7 +873,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="M38" s="1" t="s">
         <v>4</v>
       </c>
@@ -877,7 +884,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f>2.74^12</f>
+        <v>179063.37005042622</v>
+      </c>
       <c r="M39" s="1" t="s">
         <v>5</v>
       </c>
@@ -888,24 +899,24 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="O40">
         <f>SUM(O34:O39)</f>
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="44" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="N44">
         <f>0.65/2</f>
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="46" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L46" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="M47" s="1" t="s">
         <v>2</v>
       </c>
@@ -916,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="M48" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +938,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="49" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
       <c r="M49" s="1" t="s">
         <v>1</v>
       </c>
@@ -938,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
       <c r="M50" s="1" t="s">
         <v>3</v>
       </c>
@@ -949,7 +960,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="51" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
       <c r="M51" s="1" t="s">
         <v>4</v>
       </c>
@@ -960,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
       <c r="M52" s="1" t="s">
         <v>5</v>
       </c>
@@ -971,10 +982,85 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="53" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
       <c r="O53">
         <f>SUM(O47:O52)</f>
         <v>0.64999999999999991</v>
+      </c>
+    </row>
+    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L56" t="s">
+        <v>11</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N56" s="3">
+        <v>0.1588</v>
+      </c>
+      <c r="O56">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="M57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N57" s="3">
+        <v>0.1134</v>
+      </c>
+      <c r="O57">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="M58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N58" s="3">
+        <v>0.1326</v>
+      </c>
+      <c r="O58">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="M59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N59" s="3">
+        <v>0.1101</v>
+      </c>
+      <c r="O59">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="M60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N60" s="3">
+        <v>0.1323</v>
+      </c>
+      <c r="O60">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="61" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="M61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N61" s="3">
+        <v>0.1113</v>
+      </c>
+      <c r="O61">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="62" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <f>SUM(O56:O61)</f>
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code with feature selection and PCA
</commit_message>
<xml_diff>
--- a/ponderacion_modelos.xlsx
+++ b/ponderacion_modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malfaro\Desktop\mae_code\House_price_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE3EF52-FF53-4AE1-8EE3-D1E0DB7543EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7928D1-4B96-4983-B16B-210BED40B4F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14785086-4257-45D9-9F19-8FF5E0E725A2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
   <si>
     <t>lightgbm</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>all_2</t>
+  </si>
+  <si>
+    <t>train_mae</t>
   </si>
 </sst>
 </file>
@@ -442,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F149A9AD-B57D-46C1-8C8B-66C5A0940566}">
   <dimension ref="B3:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="P62" sqref="P62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +941,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M49" s="1" t="s">
         <v>1</v>
       </c>
@@ -949,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M50" s="1" t="s">
         <v>3</v>
       </c>
@@ -960,7 +963,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M51" s="1" t="s">
         <v>4</v>
       </c>
@@ -971,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M52" s="1" t="s">
         <v>5</v>
       </c>
@@ -982,13 +985,25 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O53">
         <f>SUM(O47:O52)</f>
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <v>5.3E-3</v>
+      </c>
+      <c r="E56">
+        <v>0.1</v>
+      </c>
       <c r="L56" t="s">
         <v>11</v>
       </c>
@@ -1002,7 +1017,16 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3">
+        <v>5.62E-2</v>
+      </c>
+      <c r="E57">
+        <v>0.05</v>
+      </c>
       <c r="M57" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1037,16 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E58">
+        <v>0.1</v>
+      </c>
       <c r="M58" s="1" t="s">
         <v>1</v>
       </c>
@@ -1024,7 +1057,16 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="59" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0.25</v>
+      </c>
       <c r="M59" s="1" t="s">
         <v>3</v>
       </c>
@@ -1035,7 +1077,16 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="60" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="3">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.1</v>
+      </c>
       <c r="M60" s="1" t="s">
         <v>4</v>
       </c>
@@ -1046,7 +1097,16 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="61" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="E61">
+        <v>0.05</v>
+      </c>
       <c r="M61" s="1" t="s">
         <v>5</v>
       </c>
@@ -1057,7 +1117,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <f>SUM(E56:E61)</f>
+        <v>0.65</v>
+      </c>
       <c r="O62">
         <f>SUM(O56:O61)</f>
         <v>0.65</v>

</xml_diff>